<commit_message>
update: schema, editor, examples
</commit_message>
<xml_diff>
--- a/examples/format-basic/data-file.xlsx
+++ b/examples/format-basic/data-file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nils/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulrike/Documents/Git/fx-reports-dev/examples/format-basic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BE4442-071B-D741-A1AB-557A6D7044D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325D4D4E-4C8D-8F4A-B2E6-6D67A4212F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16500" yWindow="460" windowWidth="28980" windowHeight="24620" xr2:uid="{ABF01E32-404C-4E4C-8596-6F7EA313BDFC}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="FakeNameGenerator.com_e6cf4fc0" localSheetId="0">Tabelle1!$A$1:$AS$10</definedName>
+    <definedName name="FakeNameGenerator.com_e6cf4fc0" localSheetId="0">Tabelle1!$B$1:$AS$10</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -2505,17 +2505,17 @@
   <dimension ref="A1:AS27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD27"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.6640625" bestFit="1" customWidth="1"/>
@@ -2557,22 +2557,22 @@
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
@@ -2693,23 +2693,23 @@
       </c>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>46</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>47</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
       </c>
       <c r="G2" t="s">
         <v>50</v>
@@ -2827,23 +2827,23 @@
       </c>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>76</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>77</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>78</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>79</v>
-      </c>
-      <c r="F3" t="s">
-        <v>80</v>
       </c>
       <c r="G3" t="s">
         <v>81</v>
@@ -2955,23 +2955,23 @@
       </c>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>45</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>104</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>47</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>105</v>
-      </c>
-      <c r="F4" t="s">
-        <v>106</v>
       </c>
       <c r="G4" t="s">
         <v>107</v>
@@ -3089,23 +3089,23 @@
       </c>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>76</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>133</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>78</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>134</v>
-      </c>
-      <c r="F5" t="s">
-        <v>135</v>
       </c>
       <c r="G5" t="s">
         <v>136</v>
@@ -3217,23 +3217,23 @@
       </c>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>160</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>47</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>161</v>
-      </c>
-      <c r="F6" t="s">
-        <v>162</v>
       </c>
       <c r="G6" t="s">
         <v>163</v>
@@ -3351,23 +3351,23 @@
       </c>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>45</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>186</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>47</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>187</v>
-      </c>
-      <c r="F7" t="s">
-        <v>188</v>
       </c>
       <c r="G7" t="s">
         <v>189</v>
@@ -3482,23 +3482,23 @@
       </c>
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>76</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>211</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>212</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>213</v>
-      </c>
-      <c r="F8" t="s">
-        <v>214</v>
       </c>
       <c r="G8" t="s">
         <v>215</v>
@@ -3619,23 +3619,23 @@
       </c>
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" t="s">
+        <v>242</v>
+      </c>
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>76</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>240</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>78</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>241</v>
-      </c>
-      <c r="F9" t="s">
-        <v>242</v>
       </c>
       <c r="G9" t="s">
         <v>243</v>
@@ -3756,23 +3756,23 @@
       </c>
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" t="s">
+        <v>271</v>
+      </c>
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>76</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>269</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>78</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>270</v>
-      </c>
-      <c r="F10" t="s">
-        <v>271</v>
       </c>
       <c r="G10" t="s">
         <v>272</v>
@@ -3884,23 +3884,23 @@
       </c>
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>45</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>291</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>47</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>292</v>
-      </c>
-      <c r="F11" t="s">
-        <v>135</v>
       </c>
       <c r="G11" t="s">
         <v>293</v>
@@ -4021,23 +4021,23 @@
       </c>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" t="s">
+        <v>315</v>
+      </c>
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>133</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>47</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>314</v>
-      </c>
-      <c r="F12" t="s">
-        <v>315</v>
       </c>
       <c r="G12" t="s">
         <v>316</v>
@@ -4155,23 +4155,23 @@
       </c>
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" t="s">
+        <v>342</v>
+      </c>
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>76</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>340</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>212</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>341</v>
-      </c>
-      <c r="F13" t="s">
-        <v>342</v>
       </c>
       <c r="G13" t="s">
         <v>343</v>
@@ -4292,23 +4292,23 @@
       </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" t="s">
+        <v>214</v>
+      </c>
+      <c r="B14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>45</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>364</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>47</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>365</v>
-      </c>
-      <c r="F14" t="s">
-        <v>214</v>
       </c>
       <c r="G14" t="s">
         <v>366</v>
@@ -4426,23 +4426,23 @@
       </c>
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" t="s">
+        <v>390</v>
+      </c>
+      <c r="B15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>45</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>269</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>47</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>389</v>
-      </c>
-      <c r="F15" t="s">
-        <v>390</v>
       </c>
       <c r="G15" t="s">
         <v>391</v>
@@ -4554,23 +4554,23 @@
       </c>
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" t="s">
+        <v>342</v>
+      </c>
+      <c r="B16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>45</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>411</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>47</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>412</v>
-      </c>
-      <c r="F16" t="s">
-        <v>342</v>
       </c>
       <c r="G16" t="s">
         <v>413</v>
@@ -4691,23 +4691,23 @@
       </c>
     </row>
     <row r="17" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" t="s">
+        <v>439</v>
+      </c>
+      <c r="B17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>45</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>437</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>47</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>438</v>
-      </c>
-      <c r="F17" t="s">
-        <v>439</v>
       </c>
       <c r="G17" t="s">
         <v>440</v>
@@ -4828,23 +4828,23 @@
       </c>
     </row>
     <row r="18" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" t="s">
+        <v>465</v>
+      </c>
+      <c r="B18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>45</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>463</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>47</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>464</v>
-      </c>
-      <c r="F18" t="s">
-        <v>465</v>
       </c>
       <c r="G18" t="s">
         <v>466</v>
@@ -4965,23 +4965,23 @@
       </c>
     </row>
     <row r="19" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" t="s">
+        <v>491</v>
+      </c>
+      <c r="B19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>76</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>211</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>78</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>490</v>
-      </c>
-      <c r="F19" t="s">
-        <v>491</v>
       </c>
       <c r="G19" t="s">
         <v>492</v>
@@ -5093,23 +5093,23 @@
       </c>
     </row>
     <row r="20" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" t="s">
+        <v>242</v>
+      </c>
+      <c r="B20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>45</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>510</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>47</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>511</v>
-      </c>
-      <c r="F20" t="s">
-        <v>242</v>
       </c>
       <c r="G20" t="s">
         <v>512</v>
@@ -5230,23 +5230,23 @@
       </c>
     </row>
     <row r="21" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" t="s">
+        <v>315</v>
+      </c>
+      <c r="B21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>45</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>240</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>47</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>533</v>
-      </c>
-      <c r="F21" t="s">
-        <v>315</v>
       </c>
       <c r="G21" t="s">
         <v>534</v>
@@ -5364,23 +5364,23 @@
       </c>
     </row>
     <row r="22" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" t="s">
+        <v>465</v>
+      </c>
+      <c r="B22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>45</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>340</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>47</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>554</v>
-      </c>
-      <c r="F22" t="s">
-        <v>465</v>
       </c>
       <c r="G22" t="s">
         <v>555</v>
@@ -5498,23 +5498,23 @@
       </c>
     </row>
     <row r="23" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" t="s">
+        <v>188</v>
+      </c>
+      <c r="B23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>76</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>577</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>78</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>578</v>
-      </c>
-      <c r="F23" t="s">
-        <v>188</v>
       </c>
       <c r="G23" t="s">
         <v>579</v>
@@ -5629,23 +5629,23 @@
       </c>
     </row>
     <row r="24" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" t="s">
+        <v>465</v>
+      </c>
+      <c r="B24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>76</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>364</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>212</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>598</v>
-      </c>
-      <c r="F24" t="s">
-        <v>465</v>
       </c>
       <c r="G24" t="s">
         <v>599</v>
@@ -5763,23 +5763,23 @@
       </c>
     </row>
     <row r="25" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" t="s">
+        <v>623</v>
+      </c>
+      <c r="B25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>76</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>269</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>212</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>622</v>
-      </c>
-      <c r="F25" t="s">
-        <v>623</v>
       </c>
       <c r="G25" t="s">
         <v>624</v>
@@ -5894,23 +5894,23 @@
       </c>
     </row>
     <row r="26" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>76</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>133</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>78</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>644</v>
-      </c>
-      <c r="F26" t="s">
-        <v>135</v>
       </c>
       <c r="G26" t="s">
         <v>645</v>
@@ -6031,23 +6031,23 @@
       </c>
     </row>
     <row r="27" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" t="s">
+        <v>664</v>
+      </c>
+      <c r="B27">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>76</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>46</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>78</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>663</v>
-      </c>
-      <c r="F27" t="s">
-        <v>664</v>
       </c>
       <c r="G27" t="s">
         <v>665</v>
@@ -6163,5 +6163,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>